<commit_message>
Final Stable Commit : EDA Completed
</commit_message>
<xml_diff>
--- a/Credit Card Data.xlsx
+++ b/Credit Card Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5944fdb21f69ad30/Desktop/GitHub/EDA-for-Credit-Card-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_A846A3205945C211849B71443B91C8B19B4BB9BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A846A3205945C211849B71443B91C8B19B4BB9BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19E9C065-93A2-4291-86F1-69A8E3D18FB9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Acqusition" sheetId="1" r:id="rId1"/>
@@ -1012,8 +1012,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1061,8 +1061,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="11">
-        <f ca="1">RAND()*80</f>
-        <v>19.389224387222281</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
         <v>106</v>
@@ -1088,8 +1087,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="11">
-        <f t="shared" ref="C3:C66" ca="1" si="0">RAND()*80</f>
-        <v>27.422015889786231</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
         <v>163</v>
@@ -1115,8 +1113,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>76.317326737350484</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>107</v>
@@ -1142,8 +1139,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>69.11712486475578</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>108</v>
@@ -1169,8 +1165,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>43.681078909404633</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>106</v>
@@ -1196,8 +1191,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>47.170367003358891</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
         <v>109</v>
@@ -1223,8 +1217,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>16.897704948385783</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>107</v>
@@ -1250,8 +1243,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>59.680950731276639</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
         <v>110</v>
@@ -1277,8 +1269,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>62.64385003975783</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
         <v>111</v>
@@ -1304,8 +1295,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>77.22582484646226</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>163</v>
@@ -1331,8 +1321,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>30.770749033061911</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>107</v>
@@ -1358,8 +1347,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>37.800261789612463</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
         <v>108</v>
@@ -1385,8 +1373,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>52.943469361122226</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>106</v>
@@ -1412,8 +1399,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>48.313388028749465</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>106</v>
@@ -1439,8 +1425,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>17.771334267565734</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
         <v>163</v>
@@ -1466,8 +1451,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>12.305713190193286</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>107</v>
@@ -1493,8 +1477,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7475973998887415</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
         <v>108</v>
@@ -1520,8 +1503,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>34.569903896387999</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
         <v>106</v>
@@ -1547,8 +1529,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>15.79464361804594</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
         <v>106</v>
@@ -1574,8 +1555,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>58.209974020952345</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
         <v>163</v>
@@ -1601,8 +1581,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>59.661888686749982</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
         <v>107</v>
@@ -1628,8 +1607,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>58.465730918673131</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
         <v>108</v>
@@ -1655,8 +1633,7 @@
         <v>28</v>
       </c>
       <c r="C24" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>55.420452128130719</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
         <v>106</v>
@@ -1682,8 +1659,7 @@
         <v>29</v>
       </c>
       <c r="C25" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>69.467458621608415</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
         <v>109</v>
@@ -1709,8 +1685,7 @@
         <v>30</v>
       </c>
       <c r="C26" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>62.159747792100468</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
         <v>107</v>
@@ -1736,8 +1711,7 @@
         <v>31</v>
       </c>
       <c r="C27" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>64.538159352169103</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
         <v>110</v>
@@ -1763,8 +1737,7 @@
         <v>32</v>
       </c>
       <c r="C28" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>77.972012340836045</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
         <v>111</v>
@@ -1790,8 +1763,7 @@
         <v>33</v>
       </c>
       <c r="C29" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>53.702215928448815</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
         <v>112</v>
@@ -1817,8 +1789,7 @@
         <v>34</v>
       </c>
       <c r="C30" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>47.816991621943004</v>
+        <v>72</v>
       </c>
       <c r="D30" t="s">
         <v>163</v>
@@ -1844,8 +1815,7 @@
         <v>35</v>
       </c>
       <c r="C31" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>21.906834851973365</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
         <v>106</v>
@@ -1871,8 +1841,7 @@
         <v>36</v>
       </c>
       <c r="C32" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>41.64605636252962</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
         <v>163</v>
@@ -1898,8 +1867,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>20.279754014721256</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
         <v>107</v>
@@ -1925,8 +1893,7 @@
         <v>38</v>
       </c>
       <c r="C34" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>59.62136566890247</v>
+        <v>19</v>
       </c>
       <c r="D34" t="s">
         <v>108</v>
@@ -1952,8 +1919,7 @@
         <v>39</v>
       </c>
       <c r="C35" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.5855933360726127</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
         <v>163</v>
@@ -1979,8 +1945,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>15.874091740941259</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
         <v>107</v>
@@ -2006,8 +1971,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>43.519180825684877</v>
+        <v>60</v>
       </c>
       <c r="D37" t="s">
         <v>108</v>
@@ -2033,8 +1997,7 @@
         <v>42</v>
       </c>
       <c r="C38" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>34.813824302211039</v>
+        <v>61</v>
       </c>
       <c r="D38" t="s">
         <v>106</v>
@@ -2060,8 +2023,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>69.145715566959339</v>
+        <v>47</v>
       </c>
       <c r="D39" t="s">
         <v>111</v>
@@ -2087,8 +2049,7 @@
         <v>44</v>
       </c>
       <c r="C40" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9327782521571315</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
         <v>112</v>
@@ -2114,8 +2075,7 @@
         <v>45</v>
       </c>
       <c r="C41" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>43.272534347035744</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
         <v>163</v>
@@ -2141,8 +2101,7 @@
         <v>46</v>
       </c>
       <c r="C42" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>16.468641573191512</v>
+        <v>13</v>
       </c>
       <c r="D42" t="s">
         <v>107</v>
@@ -2168,8 +2127,7 @@
         <v>47</v>
       </c>
       <c r="C43" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>28.09913867107916</v>
+        <v>50</v>
       </c>
       <c r="D43" t="s">
         <v>108</v>
@@ -2195,8 +2153,7 @@
         <v>48</v>
       </c>
       <c r="C44" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>31.665832948546615</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
         <v>106</v>
@@ -2222,8 +2179,7 @@
         <v>49</v>
       </c>
       <c r="C45" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>41.142654910220166</v>
+        <v>28</v>
       </c>
       <c r="D45" t="s">
         <v>109</v>
@@ -2249,8 +2205,7 @@
         <v>50</v>
       </c>
       <c r="C46" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>77.159871263386137</v>
+        <v>67</v>
       </c>
       <c r="D46" t="s">
         <v>107</v>
@@ -2276,8 +2231,7 @@
         <v>51</v>
       </c>
       <c r="C47" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>45.2307898166341</v>
+        <v>49</v>
       </c>
       <c r="D47" t="s">
         <v>110</v>
@@ -2303,8 +2257,7 @@
         <v>52</v>
       </c>
       <c r="C48" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.9774798735105854</v>
+        <v>28</v>
       </c>
       <c r="D48" t="s">
         <v>111</v>
@@ -2330,8 +2283,7 @@
         <v>53</v>
       </c>
       <c r="C49" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>13.945002551593548</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
         <v>112</v>
@@ -2357,8 +2309,7 @@
         <v>54</v>
       </c>
       <c r="C50" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>36.001052310520585</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
         <v>163</v>
@@ -2384,8 +2335,7 @@
         <v>55</v>
       </c>
       <c r="C51" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>22.504907228251881</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
         <v>107</v>
@@ -2411,8 +2361,7 @@
         <v>56</v>
       </c>
       <c r="C52" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>25.559964912661624</v>
+        <v>59</v>
       </c>
       <c r="D52" t="s">
         <v>108</v>
@@ -2438,8 +2387,7 @@
         <v>57</v>
       </c>
       <c r="C53" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1568934677764595</v>
+        <v>50</v>
       </c>
       <c r="D53" t="s">
         <v>106</v>
@@ -2465,8 +2413,7 @@
         <v>58</v>
       </c>
       <c r="C54" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.4918848682450037</v>
+        <v>21</v>
       </c>
       <c r="D54" t="s">
         <v>109</v>
@@ -2492,8 +2439,7 @@
         <v>59</v>
       </c>
       <c r="C55" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4835900781289233</v>
+        <v>46</v>
       </c>
       <c r="D55" t="s">
         <v>107</v>
@@ -2519,8 +2465,7 @@
         <v>60</v>
       </c>
       <c r="C56" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>41.101777588923618</v>
+        <v>43</v>
       </c>
       <c r="D56" t="s">
         <v>110</v>
@@ -2546,8 +2491,7 @@
         <v>61</v>
       </c>
       <c r="C57" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>31.130518763303563</v>
+        <v>60</v>
       </c>
       <c r="D57" t="s">
         <v>111</v>
@@ -2573,8 +2517,7 @@
         <v>62</v>
       </c>
       <c r="C58" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>30.652155988483685</v>
+        <v>37</v>
       </c>
       <c r="D58" t="s">
         <v>112</v>
@@ -2600,8 +2543,7 @@
         <v>63</v>
       </c>
       <c r="C59" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>51.97042666305461</v>
+        <v>32</v>
       </c>
       <c r="D59" t="s">
         <v>163</v>
@@ -2627,8 +2569,7 @@
         <v>64</v>
       </c>
       <c r="C60" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>66.619681002146947</v>
+        <v>74</v>
       </c>
       <c r="D60" t="s">
         <v>106</v>
@@ -2654,8 +2595,7 @@
         <v>65</v>
       </c>
       <c r="C61" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>22.695639453547003</v>
+        <v>28</v>
       </c>
       <c r="D61" t="s">
         <v>163</v>
@@ -2681,8 +2621,7 @@
         <v>66</v>
       </c>
       <c r="C62" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>49.200219185642496</v>
+        <v>44</v>
       </c>
       <c r="D62" t="s">
         <v>107</v>
@@ -2708,8 +2647,7 @@
         <v>67</v>
       </c>
       <c r="C63" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>58.173449109687297</v>
+        <v>39</v>
       </c>
       <c r="D63" t="s">
         <v>108</v>
@@ -2735,8 +2673,7 @@
         <v>68</v>
       </c>
       <c r="C64" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>49.455308728963807</v>
+        <v>15</v>
       </c>
       <c r="D64" t="s">
         <v>106</v>
@@ -2762,8 +2699,7 @@
         <v>69</v>
       </c>
       <c r="C65" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>47.801700638533248</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
         <v>109</v>
@@ -2789,8 +2725,7 @@
         <v>70</v>
       </c>
       <c r="C66" s="11">
-        <f t="shared" ca="1" si="0"/>
-        <v>15.118673293549376</v>
+        <v>41</v>
       </c>
       <c r="D66" t="s">
         <v>107</v>
@@ -2816,8 +2751,7 @@
         <v>71</v>
       </c>
       <c r="C67" s="11">
-        <f t="shared" ref="C67:C100" ca="1" si="1">RAND()*80</f>
-        <v>11.658083733880238</v>
+        <v>77</v>
       </c>
       <c r="D67" t="s">
         <v>110</v>
@@ -2843,8 +2777,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>79.275438977371152</v>
+        <v>54</v>
       </c>
       <c r="D68" t="s">
         <v>111</v>
@@ -2870,8 +2803,7 @@
         <v>73</v>
       </c>
       <c r="C69" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>72.751771316759942</v>
+        <v>12</v>
       </c>
       <c r="D69" t="s">
         <v>112</v>
@@ -2897,8 +2829,7 @@
         <v>74</v>
       </c>
       <c r="C70" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>57.506884155867695</v>
+        <v>33</v>
       </c>
       <c r="D70" t="s">
         <v>163</v>
@@ -2924,8 +2855,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>56.713366950132666</v>
+        <v>16</v>
       </c>
       <c r="D71" t="s">
         <v>108</v>
@@ -2951,8 +2881,7 @@
         <v>76</v>
       </c>
       <c r="C72" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>76.063230145863102</v>
+        <v>34</v>
       </c>
       <c r="D72" t="s">
         <v>108</v>
@@ -2978,8 +2907,7 @@
         <v>77</v>
       </c>
       <c r="C73" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>19.137197093415637</v>
+        <v>63</v>
       </c>
       <c r="D73" t="s">
         <v>106</v>
@@ -3005,8 +2933,7 @@
         <v>78</v>
       </c>
       <c r="C74" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>51.042942472000796</v>
+        <v>75</v>
       </c>
       <c r="D74" t="s">
         <v>163</v>
@@ -3032,8 +2959,7 @@
         <v>79</v>
       </c>
       <c r="C75" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>66.546715522556639</v>
+        <v>51</v>
       </c>
       <c r="D75" t="s">
         <v>107</v>
@@ -3059,8 +2985,7 @@
         <v>80</v>
       </c>
       <c r="C76" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3825742652902484</v>
+        <v>36</v>
       </c>
       <c r="D76" t="s">
         <v>108</v>
@@ -3086,8 +3011,7 @@
         <v>81</v>
       </c>
       <c r="C77" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>21.942434622728193</v>
+        <v>66</v>
       </c>
       <c r="D77" t="s">
         <v>106</v>
@@ -3113,8 +3037,7 @@
         <v>82</v>
       </c>
       <c r="C78" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>29.573559061882726</v>
+        <v>35</v>
       </c>
       <c r="D78" t="s">
         <v>106</v>
@@ -3140,8 +3063,7 @@
         <v>83</v>
       </c>
       <c r="C79" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>41.933385187389831</v>
+        <v>71</v>
       </c>
       <c r="D79" t="s">
         <v>163</v>
@@ -3167,8 +3089,7 @@
         <v>84</v>
       </c>
       <c r="C80" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>63.112839553785832</v>
+        <v>60</v>
       </c>
       <c r="D80" t="s">
         <v>107</v>
@@ -3194,8 +3115,7 @@
         <v>85</v>
       </c>
       <c r="C81" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>14.378975474723115</v>
+        <v>39</v>
       </c>
       <c r="D81" t="s">
         <v>108</v>
@@ -3221,8 +3141,7 @@
         <v>86</v>
       </c>
       <c r="C82" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>36.5968800140271</v>
+        <v>65</v>
       </c>
       <c r="D82" t="s">
         <v>106</v>
@@ -3248,8 +3167,7 @@
         <v>87</v>
       </c>
       <c r="C83" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>16.602249168728918</v>
+        <v>52</v>
       </c>
       <c r="D83" t="s">
         <v>109</v>
@@ -3275,8 +3193,7 @@
         <v>88</v>
       </c>
       <c r="C84" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>34.855481219982245</v>
+        <v>37</v>
       </c>
       <c r="D84" t="s">
         <v>107</v>
@@ -3302,8 +3219,7 @@
         <v>89</v>
       </c>
       <c r="C85" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>67.636036444788616</v>
+        <v>70</v>
       </c>
       <c r="D85" t="s">
         <v>110</v>
@@ -3329,8 +3245,7 @@
         <v>90</v>
       </c>
       <c r="C86" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>69.162147328278309</v>
+        <v>59</v>
       </c>
       <c r="D86" t="s">
         <v>111</v>
@@ -3356,8 +3271,7 @@
         <v>91</v>
       </c>
       <c r="C87" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>55.029030614513175</v>
+        <v>25</v>
       </c>
       <c r="D87" t="s">
         <v>112</v>
@@ -3383,8 +3297,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>69.820824652457773</v>
+        <v>27</v>
       </c>
       <c r="D88" t="s">
         <v>163</v>
@@ -3410,8 +3323,7 @@
         <v>93</v>
       </c>
       <c r="C89" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>60.198232593226876</v>
+        <v>63</v>
       </c>
       <c r="D89" t="s">
         <v>106</v>
@@ -3437,8 +3349,7 @@
         <v>94</v>
       </c>
       <c r="C90" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>29.022163712526723</v>
+        <v>72</v>
       </c>
       <c r="D90" t="s">
         <v>163</v>
@@ -3464,8 +3375,7 @@
         <v>95</v>
       </c>
       <c r="C91" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>17.483572398719982</v>
+        <v>16</v>
       </c>
       <c r="D91" t="s">
         <v>107</v>
@@ -3491,8 +3401,7 @@
         <v>96</v>
       </c>
       <c r="C92" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>54.179304062217284</v>
+        <v>41</v>
       </c>
       <c r="D92" t="s">
         <v>108</v>
@@ -3518,8 +3427,7 @@
         <v>97</v>
       </c>
       <c r="C93" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.67485909793973953</v>
+        <v>78</v>
       </c>
       <c r="D93" t="s">
         <v>106</v>
@@ -3545,8 +3453,7 @@
         <v>98</v>
       </c>
       <c r="C94" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>25.8686136821707</v>
+        <v>56</v>
       </c>
       <c r="D94" t="s">
         <v>109</v>
@@ -3572,8 +3479,7 @@
         <v>99</v>
       </c>
       <c r="C95" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>19.601326260472103</v>
+        <v>31</v>
       </c>
       <c r="D95" t="s">
         <v>107</v>
@@ -3599,8 +3505,7 @@
         <v>100</v>
       </c>
       <c r="C96" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>70.151872097299417</v>
+        <v>62</v>
       </c>
       <c r="D96" t="s">
         <v>110</v>
@@ -3626,8 +3531,7 @@
         <v>101</v>
       </c>
       <c r="C97" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>31.927363122138761</v>
+        <v>54</v>
       </c>
       <c r="D97" t="s">
         <v>111</v>
@@ -3653,8 +3557,7 @@
         <v>102</v>
       </c>
       <c r="C98" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>29.202575959523884</v>
+        <v>58</v>
       </c>
       <c r="D98" t="s">
         <v>112</v>
@@ -3680,8 +3583,7 @@
         <v>103</v>
       </c>
       <c r="C99" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>64.651130397215468</v>
+        <v>51</v>
       </c>
       <c r="D99" t="s">
         <v>163</v>
@@ -3707,8 +3609,7 @@
         <v>104</v>
       </c>
       <c r="C100" s="11">
-        <f t="shared" ca="1" si="1"/>
-        <v>66.162639765561323</v>
+        <v>35</v>
       </c>
       <c r="D100" t="s">
         <v>163</v>
@@ -3734,8 +3635,7 @@
         <v>105</v>
       </c>
       <c r="C101" s="11">
-        <f ca="1">RAND()*80</f>
-        <v>34.697342166351831</v>
+        <v>36</v>
       </c>
       <c r="D101" t="s">
         <v>107</v>
@@ -29307,7 +29207,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E1524"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>